<commit_message>
Limiting Reagent treatment + altered family conservation
Code is still in progress but wanted to commit now. Major changes:

 - Changed commenting and otherwise cleaned the Halogen mechanisms
 - Added ability to parallelize calc_HybridJtables.m
 - Added another J-value (Jn51, IBr)
 - Added code for limiting reagent reactions in ModelCore, dydt_eval, and Jac_eval
 - Changed family conservation to use a simple dydt "leak plug" instead of mass matrix. The latter has issues with large families as output depends on which species is used for conservation. The new method works OK but Jac_eval still has issues with larger families . . . the Jacobian is ugly and it's possible I coded it wrong. Jacobian is commented out in IntegrateStep.m for now.

The issue with the Jacobian needs to be resolved, OR I could try mass matrix again but with non-singular mass matrices (values at non-diagonals). More experiments await.
</commit_message>
<xml_diff>
--- a/Chem/Photolysis/PhotoDataSources.xlsx
+++ b/Chem/Photolysis/PhotoDataSources.xlsx
@@ -15,12 +15,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="356">
   <si>
     <t>Mechanism Names</t>
   </si>
@@ -1079,6 +1078,15 @@
   </si>
   <si>
     <t>Cross_Section_ICl_JPL-2010(2011)_298K_210-600nm(rec).txt</t>
+  </si>
+  <si>
+    <t>Ibr</t>
+  </si>
+  <si>
+    <t>Jn51</t>
+  </si>
+  <si>
+    <t>Cross_Section_IBr_JPL-2010(2011)_298K_220-600nm(rec).txt</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1662,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D28" sqref="D28"/>
+      <selection pane="topRight" activeCell="K91" sqref="K91:M91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -4669,19 +4677,31 @@
       </c>
     </row>
     <row r="91" spans="1:13">
-      <c r="A91" s="1"/>
-      <c r="B91" s="3"/>
+      <c r="A91" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>354</v>
+      </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="5"/>
+      <c r="G91" s="5" t="s">
+        <v>355</v>
+      </c>
       <c r="H91" s="5"/>
-      <c r="I91" s="6"/>
+      <c r="I91" s="46">
+        <v>43466</v>
+      </c>
       <c r="J91" s="1"/>
-      <c r="K91" s="8"/>
+      <c r="K91" s="8">
+        <v>1</v>
+      </c>
       <c r="L91" s="8"/>
-      <c r="M91" s="8"/>
+      <c r="M91" s="46">
+        <v>43466</v>
+      </c>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="1"/>

</xml_diff>

<commit_message>
Addition of NOAA BB Mechanism and minor photolysis rejiggering
 - Added NOAA BB Mechanism
 - Added Jn52 to J_BottomUp.m and regenerated HybridJtables.mat
 - Moved acquisition of hybrid J-values for non-MCM photolysis into MCMv331_J.m and out of *_J.m files for other mechanisms. This allows MCM submechanisms to be used with any of the J parameterization options.
 - Minor bug fix in F0AM_ModelCore for SolarParam.resetConcDaily default value (nan to 0)
 - Updated user manual and change log.
</commit_message>
<xml_diff>
--- a/Chem/Photolysis/PhotoDataSources.xlsx
+++ b/Chem/Photolysis/PhotoDataSources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GMWfiles\F0AM\F0AMv4\Chem\Photolysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GMWFiles\F0AM\F0AM_git\Chem\Photolysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="361">
   <si>
     <t>Mechanism Names</t>
   </si>
@@ -1080,13 +1080,28 @@
     <t>Cross_Section_ICl_JPL-2010(2011)_298K_210-600nm(rec).txt</t>
   </si>
   <si>
-    <t>Ibr</t>
-  </si>
-  <si>
     <t>Jn51</t>
   </si>
   <si>
     <t>Cross_Section_IBr_JPL-2010(2011)_298K_220-600nm(rec).txt</t>
+  </si>
+  <si>
+    <t>IBr</t>
+  </si>
+  <si>
+    <t>Jn52</t>
+  </si>
+  <si>
+    <t>Cross_Section_FURFURAL.csv</t>
+  </si>
+  <si>
+    <t>FURFURAL</t>
+  </si>
+  <si>
+    <t>MPI-MAINZ</t>
+  </si>
+  <si>
+    <t>M. Coggon, personal communication, 2019</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1353,6 +1368,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1660,9 +1680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K91" sqref="K91:M91"/>
+      <selection pane="topRight" activeCell="M94" sqref="M94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -4678,17 +4698,17 @@
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>354</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="1"/>
       <c r="G91" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H91" s="5"/>
       <c r="I91" s="46">
@@ -4719,19 +4739,35 @@
       <c r="M92" s="8"/>
     </row>
     <row r="93" spans="1:13">
-      <c r="A93" s="1"/>
-      <c r="B93" s="3"/>
+      <c r="A93" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>356</v>
+      </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="5"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="6"/>
+      <c r="G93" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="H93" s="49" t="s">
+        <v>359</v>
+      </c>
+      <c r="I93" s="50">
+        <v>43586</v>
+      </c>
       <c r="J93" s="1"/>
-      <c r="K93" s="8"/>
-      <c r="L93" s="8"/>
-      <c r="M93" s="8"/>
+      <c r="K93" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="L93" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="M93" s="51">
+        <v>43586</v>
+      </c>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="1"/>
@@ -18437,8 +18473,9 @@
     <hyperlink ref="L3" r:id="rId65"/>
     <hyperlink ref="L35" r:id="rId66"/>
     <hyperlink ref="L22" r:id="rId67"/>
+    <hyperlink ref="H93" r:id="rId68"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId68"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId69"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v4.1.2: Big bug fix for PlotRates.m, minor fixes for photolysis
Cross_Section_4_methyl_2_nitrophenol.csv: replaced negative values with 0. Thanks to Eleanora Puppolola.
Cross_Section_PAN.csv: removed some rows with missing data.
IntegrateJ.m: Changed error messages to warnings (still throws error if nan/neg)
		Added filename text to plots
		Added warnings for negative LF/QY/CS and removed a line that corrected negative LF to 0.
PlotRates.m: Fixed bug in family reaction summation, so that family cross reactions are now properly accounted for.
		For example, LROx(CH3O2 + HO2) = 2*rate(CH3O2 + HO2) = LCH3O2 + LHO2.
</commit_message>
<xml_diff>
--- a/Chem/Photolysis/PhotoDataSources.xlsx
+++ b/Chem/Photolysis/PhotoDataSources.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GMWFiles\F0AM\F0AMv4\Chem\Photolysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GMWFiles\F0AM\F0AMdev\Chem\Photolysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="408">
   <si>
     <t>Mechanism Names</t>
   </si>
@@ -582,9 +582,6 @@
     <t>Quantum_Yield_Acrolein.m</t>
   </si>
   <si>
-    <t>Cross_Section_3_methy_2_nitrophenol.csv; 4_methyl_2_nitrophenol.csv</t>
-  </si>
-  <si>
     <t>JPAN</t>
   </si>
   <si>
@@ -1240,6 +1237,12 @@
   </si>
   <si>
     <t>JNPRNO3</t>
+  </si>
+  <si>
+    <t>Cross_Section_4_methyl_2_nitrophenol.csv</t>
+  </si>
+  <si>
+    <t>Cross_Section_3_methy_2_nitrophenol.csv</t>
   </si>
 </sst>
 </file>
@@ -1819,9 +1822,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F34" sqref="F34"/>
+      <selection pane="topRight" activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1870,7 +1873,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="P1" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1887,7 +1890,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -1913,10 +1916,10 @@
         <v>10</v>
       </c>
       <c r="P2" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q2" s="15" t="s">
         <v>237</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1933,7 +1936,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
@@ -1943,7 +1946,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J3" s="17">
         <v>42422</v>
@@ -1953,7 +1956,7 @@
         <v>15</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N3" s="19">
         <v>42422</v>
@@ -1979,7 +1982,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>18</v>
@@ -2029,7 +2032,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J5" s="6">
         <v>2012</v>
@@ -2059,7 +2062,7 @@
         <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>26</v>
@@ -2069,7 +2072,7 @@
         <v>27</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J6" s="6">
         <v>2012</v>
@@ -2079,7 +2082,7 @@
         <v>28</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N6" s="8">
         <v>2012</v>
@@ -2105,7 +2108,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>31</v>
@@ -2115,7 +2118,7 @@
         <v>32</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J7" s="6">
         <v>2012</v>
@@ -2125,7 +2128,7 @@
         <v>33</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N7" s="8">
         <v>2012</v>
@@ -2151,7 +2154,7 @@
         <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>36</v>
@@ -2165,7 +2168,7 @@
         <v>37</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N8" s="8">
         <v>2012</v>
@@ -2191,7 +2194,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>40</v>
@@ -2201,7 +2204,7 @@
         <v>41</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J9" s="6">
         <v>2012</v>
@@ -2241,7 +2244,7 @@
         <v>45</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J10" s="6">
         <v>2012</v>
@@ -2271,7 +2274,7 @@
         <v>49</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>49</v>
@@ -2281,7 +2284,7 @@
         <v>50</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J11" s="17">
         <v>42432</v>
@@ -2291,7 +2294,7 @@
         <v>51</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N11" s="8">
         <v>2012</v>
@@ -2317,7 +2320,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>55</v>
@@ -2331,7 +2334,7 @@
         <v>56</v>
       </c>
       <c r="M12" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N12" s="8"/>
       <c r="P12" s="20">
@@ -2343,7 +2346,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>58</v>
@@ -2365,17 +2368,17 @@
         <v>62</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J13" s="6">
         <v>2016</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="25" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N13" s="26">
         <v>42426</v>
@@ -2411,7 +2414,7 @@
         <v>68</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J14" s="6">
         <v>2016</v>
@@ -2421,7 +2424,7 @@
         <v>69</v>
       </c>
       <c r="M14" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="N14" s="8">
         <v>2016</v>
@@ -2449,23 +2452,23 @@
         <v>72</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J15" s="6">
         <v>2012</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N15" s="8">
         <v>2016</v>
       </c>
       <c r="P15" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q15" s="20">
         <v>1.1421767805785199</v>
@@ -2488,14 +2491,14 @@
       <c r="J16" s="6"/>
       <c r="K16" s="1"/>
       <c r="L16" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M16" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N16" s="8"/>
       <c r="P16" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q16" s="20">
         <v>0.90659774594889297</v>
@@ -2517,7 +2520,7 @@
         <v>77</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J17" s="6">
         <v>2016</v>
@@ -2527,13 +2530,13 @@
         <v>78</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N17" s="8">
         <v>2016</v>
       </c>
       <c r="P17" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q17" s="20">
         <v>1.8832627736113701</v>
@@ -2551,7 +2554,7 @@
         <v>81</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>81</v>
@@ -2561,7 +2564,7 @@
         <v>82</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J18" s="6">
         <v>2016</v>
@@ -2569,7 +2572,7 @@
       <c r="K18" s="1"/>
       <c r="L18" s="8"/>
       <c r="M18" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N18" s="8">
         <v>2016</v>
@@ -2593,7 +2596,7 @@
         <v>81</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>81</v>
@@ -2605,7 +2608,7 @@
       <c r="K19" s="1"/>
       <c r="L19" s="8"/>
       <c r="M19" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N19" s="8"/>
       <c r="P19" s="20">
@@ -2628,14 +2631,14 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="5" t="s">
         <v>82</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J20" s="6">
         <v>2016</v>
@@ -2643,7 +2646,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="8"/>
       <c r="M20" s="29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="N20" s="8">
         <v>2016</v>
@@ -2669,7 +2672,7 @@
         <v>91</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>90</v>
@@ -2679,7 +2682,7 @@
         <v>92</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J21" s="6">
         <v>2016</v>
@@ -2689,7 +2692,7 @@
         <v>93</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N21" s="8">
         <v>2016</v>
@@ -2715,7 +2718,7 @@
         <v>96</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>96</v>
@@ -2725,7 +2728,7 @@
         <v>97</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J22" s="6">
         <v>2012</v>
@@ -2735,7 +2738,7 @@
         <v>0.34</v>
       </c>
       <c r="M22" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N22" s="8">
         <v>2016</v>
@@ -2759,7 +2762,7 @@
         <v>100</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>100</v>
@@ -2769,7 +2772,7 @@
         <v>101</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J23" s="6">
         <v>2012</v>
@@ -2779,7 +2782,7 @@
         <v>102</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N23" s="8">
         <v>2012</v>
@@ -2803,7 +2806,7 @@
         <v>100</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>100</v>
@@ -2837,7 +2840,7 @@
         <v>108</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>109</v>
@@ -2847,17 +2850,17 @@
         <v>110</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J25" s="17">
         <v>42432</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="29" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M25" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N25" s="19">
         <v>42432</v>
@@ -2883,7 +2886,7 @@
         <v>113</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>109</v>
@@ -2894,10 +2897,10 @@
       <c r="J26" s="6"/>
       <c r="K26" s="1"/>
       <c r="L26" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M26" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N26" s="19">
         <v>42432</v>
@@ -2923,7 +2926,7 @@
         <v>116</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>117</v>
@@ -2934,10 +2937,10 @@
       <c r="J27" s="6"/>
       <c r="K27" s="1"/>
       <c r="L27" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M27" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N27" s="19">
         <v>42432</v>
@@ -2963,7 +2966,7 @@
         <v>121</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>120</v>
@@ -2973,17 +2976,17 @@
         <v>122</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J28" s="6">
         <v>2016</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N28" s="19">
         <v>42432</v>
@@ -3005,7 +3008,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="1"/>
@@ -3013,7 +3016,7 @@
         <v>125</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J29" s="6">
         <v>2012</v>
@@ -3040,10 +3043,10 @@
         <v>128</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>129</v>
@@ -3053,7 +3056,7 @@
         <v>130</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J30" s="6">
         <v>2012</v>
@@ -3080,14 +3083,14 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="5" t="s">
         <v>133</v>
       </c>
       <c r="I31" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J31" s="6">
         <v>2012</v>
@@ -3114,14 +3117,14 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="5" t="s">
         <v>136</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J32" s="6">
         <v>2012</v>
@@ -3148,14 +3151,14 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="5" t="s">
         <v>139</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J33" s="6">
         <v>2012</v>
@@ -3179,23 +3182,23 @@
         <v>141</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D34" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="5" t="s">
         <v>142</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J34" s="6">
         <v>2016</v>
@@ -3205,7 +3208,7 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
       <c r="P34" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q34" s="20">
         <v>1.44734264095843</v>
@@ -3227,7 +3230,7 @@
         <v>145</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J35" s="6">
         <v>2016</v>
@@ -3237,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="M35" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N35" s="8">
         <v>2016</v>
@@ -3260,7 +3263,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="5" t="s">
@@ -3314,7 +3317,7 @@
         <v>1.18207767692265</v>
       </c>
       <c r="Q37" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3360,7 +3363,7 @@
       </c>
       <c r="C40" s="31"/>
       <c r="D40" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="31"/>
@@ -3379,10 +3382,10 @@
       <c r="M40" s="34"/>
       <c r="N40" s="34"/>
       <c r="P40" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q40" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:17">
@@ -3394,10 +3397,10 @@
       </c>
       <c r="C41" s="31"/>
       <c r="D41" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F41" s="31"/>
       <c r="G41" s="1"/>
@@ -3405,7 +3408,7 @@
         <v>159</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J41" s="36">
         <v>42424</v>
@@ -3415,10 +3418,10 @@
       <c r="M41" s="34"/>
       <c r="N41" s="37"/>
       <c r="P41" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q41" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -3430,7 +3433,7 @@
       </c>
       <c r="C42" s="31"/>
       <c r="D42" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E42" s="30"/>
       <c r="F42" s="31"/>
@@ -3449,10 +3452,10 @@
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
       <c r="P42" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q42" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -3464,10 +3467,10 @@
       </c>
       <c r="C43" s="31"/>
       <c r="D43" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F43" s="31"/>
       <c r="G43" s="1"/>
@@ -3475,7 +3478,7 @@
         <v>166</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J43" s="36">
         <v>42426</v>
@@ -3488,7 +3491,7 @@
         <v>1.0554580931828199</v>
       </c>
       <c r="Q43" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:17">
@@ -3502,24 +3505,24 @@
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="38" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="32" t="s">
         <v>168</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J44" s="36">
         <v>42426</v>
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="25" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M44" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N44" s="26">
         <v>42426</v>
@@ -3528,7 +3531,7 @@
         <v>0.97886725531007801</v>
       </c>
       <c r="Q44" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:17">
@@ -3547,34 +3550,34 @@
         <v>168</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J45" s="36">
         <v>42426</v>
       </c>
       <c r="K45" s="1"/>
       <c r="L45" s="25" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M45" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N45" s="26">
         <v>42426</v>
       </c>
       <c r="P45" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q45" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B46" s="38" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C46" s="31"/>
       <c r="D46" s="3"/>
@@ -3602,14 +3605,14 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="38" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="32" t="s">
         <v>172</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J47" s="36">
         <v>42426</v>
@@ -3619,16 +3622,16 @@
         <v>173</v>
       </c>
       <c r="M47" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N47" s="26">
         <v>42426</v>
       </c>
       <c r="P47" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q47" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -3644,14 +3647,14 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G48" s="1"/>
       <c r="H48" s="32" t="s">
         <v>177</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J48" s="33" t="s">
         <v>178</v>
@@ -3664,7 +3667,7 @@
         <v>0.88398068038326105</v>
       </c>
       <c r="Q48" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:17">
@@ -3678,14 +3681,14 @@
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
       <c r="F49" s="38" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="32" t="s">
         <v>181</v>
       </c>
       <c r="I49" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J49" s="33" t="s">
         <v>178</v>
@@ -3698,7 +3701,7 @@
         <v>1.0011020640972701</v>
       </c>
       <c r="Q49" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -3713,7 +3716,7 @@
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F50" s="31"/>
       <c r="G50" s="1"/>
@@ -3721,7 +3724,7 @@
         <v>185</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J50" s="33" t="s">
         <v>178</v>
@@ -3731,7 +3734,7 @@
         <v>186</v>
       </c>
       <c r="M50" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N50" s="42">
         <v>42423</v>
@@ -3740,28 +3743,28 @@
         <v>1.0102590002521601</v>
       </c>
       <c r="Q50" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="43" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B51" s="38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="31"/>
       <c r="G51" s="1"/>
       <c r="H51" s="32" t="s">
-        <v>187</v>
+        <v>407</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J51" s="33" t="s">
         <v>178</v>
@@ -3771,27 +3774,29 @@
       <c r="M51" s="34"/>
       <c r="N51" s="34"/>
       <c r="P51" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q51" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="43" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C52" s="38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="31"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="32"/>
+      <c r="H52" s="32" t="s">
+        <v>406</v>
+      </c>
       <c r="I52" s="35"/>
       <c r="J52" s="33"/>
       <c r="K52" s="1"/>
@@ -3799,45 +3804,45 @@
       <c r="M52" s="34"/>
       <c r="N52" s="34"/>
       <c r="P52" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q52" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="43" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E53" s="30"/>
       <c r="F53" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53" s="32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J53" s="33" t="s">
         <v>178</v>
       </c>
       <c r="K53" s="1"/>
       <c r="L53" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M53" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N53" s="42">
         <v>42423</v>
@@ -3846,25 +3851,25 @@
         <v>0.91355786480184598</v>
       </c>
       <c r="Q53" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="54" spans="1:17">
       <c r="A54" s="43" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D54" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E54" s="30"/>
       <c r="F54" s="38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="32"/>
@@ -3878,28 +3883,28 @@
         <v>1.42294750549259</v>
       </c>
       <c r="Q54" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:17">
       <c r="A55" s="43" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B55" s="38" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C55" s="31"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J55" s="36">
         <v>42426</v>
@@ -3912,21 +3917,21 @@
         <v>1.0223293695723501</v>
       </c>
       <c r="Q55" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:17">
       <c r="A56" s="43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C56" s="31"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
       <c r="F56" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="32"/>
@@ -3937,18 +3942,18 @@
       <c r="M56" s="34"/>
       <c r="N56" s="34"/>
       <c r="P56" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q56" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="57" spans="1:17">
       <c r="A57" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="31" t="s">
         <v>192</v>
-      </c>
-      <c r="B57" s="31" t="s">
-        <v>193</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="3"/>
@@ -3956,10 +3961,10 @@
       <c r="F57" s="31"/>
       <c r="G57" s="1"/>
       <c r="H57" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I57" s="16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J57" s="33" t="s">
         <v>178</v>
@@ -3969,43 +3974,43 @@
       <c r="M57" s="34"/>
       <c r="N57" s="34"/>
       <c r="P57" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q57" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:17">
       <c r="A58" s="43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
       <c r="F58" s="38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J58" s="33" t="s">
         <v>178</v>
       </c>
       <c r="K58" s="1"/>
       <c r="L58" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M58" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N58" s="42">
         <v>42423</v>
@@ -4014,23 +4019,23 @@
         <v>0.941824047710492</v>
       </c>
       <c r="Q58" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="59" spans="1:17">
       <c r="A59" s="43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B59" s="38" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="32"/>
@@ -4041,33 +4046,33 @@
       <c r="M59" s="41"/>
       <c r="N59" s="42"/>
       <c r="P59" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q59" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:17">
       <c r="A60" s="43" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B60" s="38" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G60" s="1"/>
       <c r="H60" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J60" s="33" t="s">
         <v>178</v>
@@ -4080,23 +4085,23 @@
         <v>0.89281694554091795</v>
       </c>
       <c r="Q60" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:17">
       <c r="A61" s="43" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B61" s="38" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C61" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="32"/>
@@ -4110,7 +4115,7 @@
         <v>0.89281694554091795</v>
       </c>
       <c r="Q61" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -4133,23 +4138,23 @@
     </row>
     <row r="63" spans="1:17">
       <c r="A63" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B63" s="31" t="s">
         <v>199</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>200</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F63" s="31"/>
       <c r="G63" s="1"/>
       <c r="H63" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J63" s="33" t="s">
         <v>178</v>
@@ -4162,28 +4167,28 @@
         <v>0.78908947445218602</v>
       </c>
       <c r="Q63" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:17">
       <c r="A64" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B64" s="31" t="s">
         <v>202</v>
-      </c>
-      <c r="B64" s="31" t="s">
-        <v>203</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J64" s="36">
         <v>42424</v>
@@ -4196,28 +4201,28 @@
         <v>1.0186534904762199</v>
       </c>
       <c r="Q64" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="65" spans="1:17">
       <c r="A65" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" s="31" t="s">
         <v>205</v>
-      </c>
-      <c r="B65" s="31" t="s">
-        <v>206</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J65" s="36">
         <v>42424</v>
@@ -4230,28 +4235,28 @@
         <v>1.0233601873639599</v>
       </c>
       <c r="Q65" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="A66" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="B66" s="31" t="s">
         <v>208</v>
-      </c>
-      <c r="B66" s="31" t="s">
-        <v>209</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="38" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J66" s="36">
         <v>42424</v>
@@ -4264,30 +4269,30 @@
         <v>1.0585514845699</v>
       </c>
       <c r="Q66" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:17" ht="15" customHeight="1">
       <c r="A67" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B67" s="31" t="s">
         <v>211</v>
-      </c>
-      <c r="B67" s="31" t="s">
-        <v>212</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F67" s="38" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G67" s="1"/>
       <c r="H67" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J67" s="36">
         <v>42424</v>
@@ -4300,38 +4305,38 @@
         <v>1.2656475404290299</v>
       </c>
       <c r="Q67" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="15" customHeight="1">
       <c r="A68" s="43" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B68" s="38" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G68" s="1"/>
       <c r="H68" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J68" s="36">
         <v>42424</v>
       </c>
       <c r="K68" s="1"/>
       <c r="L68" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M68" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="N68" s="37">
         <v>42433</v>
@@ -4340,21 +4345,21 @@
         <v>1.0476268475311401</v>
       </c>
       <c r="Q68" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:17" ht="15" customHeight="1">
       <c r="A69" s="43" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B69" s="38" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C69" s="31"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G69" s="1"/>
       <c r="H69" s="32"/>
@@ -4368,28 +4373,28 @@
         <v>1.04753247523607</v>
       </c>
       <c r="Q69" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:17">
       <c r="A70" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G70" s="1"/>
       <c r="H70" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J70" s="36">
         <v>42424</v>
@@ -4402,15 +4407,15 @@
         <v>1.0973479197392599</v>
       </c>
       <c r="Q70" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="71" spans="1:17">
       <c r="A71" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="3"/>
@@ -4418,10 +4423,10 @@
       <c r="F71" s="31"/>
       <c r="G71" s="1"/>
       <c r="H71" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I71" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J71" s="36">
         <v>42424</v>
@@ -4434,28 +4439,28 @@
         <v>1.00284534393118</v>
       </c>
       <c r="Q71" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="72" spans="1:17">
       <c r="A72" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F72" s="31"/>
       <c r="G72" s="1"/>
       <c r="H72" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I72" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J72" s="36">
         <v>42424</v>
@@ -4468,15 +4473,15 @@
         <v>0.98890628393791202</v>
       </c>
       <c r="Q72" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="73" spans="1:17">
       <c r="A73" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="3"/>
@@ -4484,10 +4489,10 @@
       <c r="F73" s="31"/>
       <c r="G73" s="1"/>
       <c r="H73" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I73" s="44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J73" s="36">
         <v>42424</v>
@@ -4500,38 +4505,38 @@
         <v>3.6832821977160801</v>
       </c>
       <c r="Q73" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:17">
       <c r="A74" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B74" s="38" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C74" s="31"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F74" s="31"/>
       <c r="G74" s="1"/>
       <c r="H74" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J74" s="36">
         <v>42424</v>
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M74" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N74" s="26">
         <v>42424</v>
@@ -4540,20 +4545,20 @@
         <v>1.0436145227437601</v>
       </c>
       <c r="Q74" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="75" spans="1:17">
       <c r="A75" s="43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="1"/>
@@ -4568,28 +4573,28 @@
         <v>1.0852236678680101</v>
       </c>
       <c r="Q75" s="20" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="76" spans="1:17">
       <c r="A76" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B76" s="30" t="s">
         <v>271</v>
-      </c>
-      <c r="B76" s="30" t="s">
-        <v>272</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="1"/>
       <c r="H76" s="45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I76" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J76" s="36">
         <v>42424</v>
@@ -4599,7 +4604,7 @@
         <v>1</v>
       </c>
       <c r="M76" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N76" s="26">
         <v>42424</v>
@@ -4608,15 +4613,15 @@
         <v>1.0267147560158301</v>
       </c>
       <c r="Q76" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="77" spans="1:17">
       <c r="A77" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -4624,7 +4629,7 @@
       <c r="F77" s="3"/>
       <c r="G77" s="1"/>
       <c r="H77" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="46">
@@ -4641,10 +4646,10 @@
     </row>
     <row r="78" spans="1:17">
       <c r="A78" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -4652,7 +4657,7 @@
       <c r="F78" s="3"/>
       <c r="G78" s="1"/>
       <c r="H78" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="46">
@@ -4669,10 +4674,10 @@
     </row>
     <row r="79" spans="1:17">
       <c r="A79" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -4680,7 +4685,7 @@
       <c r="F79" s="3"/>
       <c r="G79" s="1"/>
       <c r="H79" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="46">
@@ -4697,10 +4702,10 @@
     </row>
     <row r="80" spans="1:17">
       <c r="A80" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3"/>
@@ -4708,7 +4713,7 @@
       <c r="F80" s="3"/>
       <c r="G80" s="1"/>
       <c r="H80" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I80" s="5"/>
       <c r="J80" s="46">
@@ -4716,7 +4721,7 @@
       </c>
       <c r="K80" s="1"/>
       <c r="L80" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M80" s="8"/>
       <c r="N80" s="46">
@@ -4725,20 +4730,20 @@
     </row>
     <row r="81" spans="1:14">
       <c r="A81" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="1"/>
       <c r="H81" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I81" s="5"/>
       <c r="J81" s="46">
@@ -4755,10 +4760,10 @@
     </row>
     <row r="82" spans="1:14">
       <c r="A82" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -4766,7 +4771,7 @@
       <c r="F82" s="3"/>
       <c r="G82" s="1"/>
       <c r="H82" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I82" s="5"/>
       <c r="J82" s="46">
@@ -4783,10 +4788,10 @@
     </row>
     <row r="83" spans="1:14">
       <c r="A83" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -4794,7 +4799,7 @@
       <c r="F83" s="3"/>
       <c r="G83" s="1"/>
       <c r="H83" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I83" s="5"/>
       <c r="J83" s="46">
@@ -4811,10 +4816,10 @@
     </row>
     <row r="84" spans="1:14">
       <c r="A84" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -4822,7 +4827,7 @@
       <c r="F84" s="3"/>
       <c r="G84" s="1"/>
       <c r="H84" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I84" s="5"/>
       <c r="J84" s="46">
@@ -4839,10 +4844,10 @@
     </row>
     <row r="85" spans="1:14">
       <c r="A85" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -4850,7 +4855,7 @@
       <c r="F85" s="3"/>
       <c r="G85" s="1"/>
       <c r="H85" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I85" s="5"/>
       <c r="J85" s="46">
@@ -4867,10 +4872,10 @@
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
@@ -4878,7 +4883,7 @@
       <c r="F86" s="3"/>
       <c r="G86" s="1"/>
       <c r="H86" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I86" s="5"/>
       <c r="J86" s="46">
@@ -4895,10 +4900,10 @@
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -4906,7 +4911,7 @@
       <c r="F87" s="3"/>
       <c r="G87" s="1"/>
       <c r="H87" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I87" s="5"/>
       <c r="J87" s="46">
@@ -4923,10 +4928,10 @@
     </row>
     <row r="88" spans="1:14">
       <c r="A88" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -4934,7 +4939,7 @@
       <c r="F88" s="3"/>
       <c r="G88" s="1"/>
       <c r="H88" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I88" s="5"/>
       <c r="J88" s="46">
@@ -4951,10 +4956,10 @@
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -4962,7 +4967,7 @@
       <c r="F89" s="3"/>
       <c r="G89" s="1"/>
       <c r="H89" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I89" s="5"/>
       <c r="J89" s="46">
@@ -4979,10 +4984,10 @@
     </row>
     <row r="90" spans="1:14">
       <c r="A90" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
@@ -4990,7 +4995,7 @@
       <c r="F90" s="3"/>
       <c r="G90" s="1"/>
       <c r="H90" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I90" s="5"/>
       <c r="J90" s="46">
@@ -5007,10 +5012,10 @@
     </row>
     <row r="91" spans="1:14">
       <c r="A91" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -5018,7 +5023,7 @@
       <c r="F91" s="3"/>
       <c r="G91" s="1"/>
       <c r="H91" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="I91" s="5"/>
       <c r="J91" s="46">
@@ -5051,10 +5056,10 @@
     </row>
     <row r="93" spans="1:14">
       <c r="A93" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -5062,10 +5067,10 @@
       <c r="F93" s="3"/>
       <c r="G93" s="1"/>
       <c r="H93" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I93" s="49" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J93" s="50">
         <v>43586</v>
@@ -5075,7 +5080,7 @@
         <v>0.5</v>
       </c>
       <c r="M93" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N93" s="51">
         <v>43586</v>
@@ -5099,23 +5104,23 @@
     </row>
     <row r="95" spans="1:14">
       <c r="A95" s="52" t="s">
+        <v>386</v>
+      </c>
+      <c r="B95" s="30" t="s">
         <v>387</v>
-      </c>
-      <c r="B95" s="30" t="s">
-        <v>388</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="1"/>
       <c r="H95" s="45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I95" s="45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J95" s="17">
         <v>43942</v>
@@ -5125,7 +5130,7 @@
         <v>1</v>
       </c>
       <c r="M95" s="29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N95" s="19">
         <v>43942</v>
@@ -5133,23 +5138,23 @@
     </row>
     <row r="96" spans="1:14">
       <c r="A96" s="52" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
       <c r="E96" s="30" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F96" s="3"/>
       <c r="G96" s="1"/>
       <c r="H96" s="45" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I96" s="45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J96" s="17">
         <v>43942</v>
@@ -5159,7 +5164,7 @@
         <v>1</v>
       </c>
       <c r="M96" s="29" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N96" s="19">
         <v>43942</v>
@@ -5167,23 +5172,23 @@
     </row>
     <row r="97" spans="1:14">
       <c r="A97" s="52" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="1"/>
       <c r="H97" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J97" s="17">
         <v>43942</v>
@@ -5199,23 +5204,23 @@
     </row>
     <row r="98" spans="1:14">
       <c r="A98" s="52" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F98" s="3"/>
       <c r="G98" s="1"/>
       <c r="H98" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J98" s="17">
         <v>43942</v>

</xml_diff>